<commit_message>
Update test CSV / Excel files: remove Missing Account # row + add Empty column
</commit_message>
<xml_diff>
--- a/tests/Staff_Parents_RosarioSIS_test.xlsx
+++ b/tests/Staff_Parents_RosarioSIS_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">Profile</t>
   </si>
   <si>
+    <t xml:space="preserve">Empty column</t>
+  </si>
+  <si>
     <t xml:space="preserve">John</t>
   </si>
   <si>
@@ -118,55 +121,46 @@
     <t xml:space="preserve">No</t>
   </si>
   <si>
-    <t xml:space="preserve">Account #</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2003-08-23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no@accountnumber.com</t>
+    <t xml:space="preserve">28-05-1984</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01.23.45.67.89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/13/05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no@pin.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teacher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123-456-789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13-05-1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13-05-1972</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no@access.com</t>
   </si>
   <si>
     <t xml:space="preserve">none</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28-05-1984</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01.23.45.67.89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05/13/05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no@pin.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teacher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123-456-789</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13-05-1989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13-05-1972</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no@access.com</t>
   </si>
 </sst>
 </file>
@@ -268,22 +262,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -311,179 +307,179 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>612345678</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>123456</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>123456789</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>123456789</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>987654321</v>
-      </c>
-      <c r="G7" s="0" t="s">
+        <v>321654987</v>
+      </c>
+      <c r="H7" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="0" t="n">
-        <v>321654987</v>
+      <c r="G8" s="0" t="s">
+        <v>37</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="0" t="s">
         <v>40</v>
       </c>
+      <c r="E9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>321654987</v>
+      </c>
       <c r="H9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>44</v>
@@ -491,28 +487,11 @@
       <c r="F10" s="0" t="n">
         <v>321654987</v>
       </c>
+      <c r="G10" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="H10" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>321654987</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>